<commit_message>
filtered by banks and by concept key
</commit_message>
<xml_diff>
--- a/data/Book6.xlsx
+++ b/data/Book6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanramirez/Library/Mobile Documents/com~apple~CloudDocs/bootcamp/Proyectos/Proyecto3/Sigma-final-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Dropbox\Personal\DataAnalytics\BootCamp\20210219_FinalProject\final\Sigma-final-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBDBD81-F859-3C40-9926-344995E4FC0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E07EC90-EB92-4FD4-BA2A-E7832ED224CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34770" yWindow="2385" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>Ingresos por intereses</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>cve_concepto</t>
+  </si>
+  <si>
+    <t>descripcion</t>
   </si>
 </sst>
 </file>
@@ -592,180 +598,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:B23"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>510000000000</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>510000000000</v>
+        <v>610000000000</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>610000000000</v>
+        <v>620000000000</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>620000000000</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>670200000000</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>670200000000</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>640000000000</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>640000000000</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>670500000000</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>670500000000</v>
+        <v>671100000000</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>671100000000</v>
+        <v>100000000000</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>110000000000</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>100000000000</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>130100000000</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>110000000000</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>130105000000</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>130100000000</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>130106000000</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>130105000000</v>
+        <v>130121000000</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>130106000000</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
+        <v>131100000000</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>130121000000</v>
+        <v>131101000000</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>131100000000</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>131199990000</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>131101000000</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>14</v>
+        <v>131600000000</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>131199990000</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>15</v>
+        <v>200000000000</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>131600000000</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>16</v>
+        <v>210100000000</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>200000000000</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1">
-        <v>210100000000</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1">
         <v>211100000000</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Bancos</formula1>
     </dataValidation>
   </dataValidations>
@@ -781,10 +795,10 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1119,10 +1133,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>